<commit_message>
pass first few tests!
</commit_message>
<xml_diff>
--- a/tests/testthat/_snaps/knitxl/file1.xlsx
+++ b/tests/testthat/_snaps/knitxl/file1.xlsx
@@ -9,6 +9,14 @@
     <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t xml:space="preserve">Some text</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -337,7 +345,13 @@
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>

</xml_diff>